<commit_message>
first round of incorporating edits for MS_v2
</commit_message>
<xml_diff>
--- a/MainTables.xlsx
+++ b/MainTables.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575"/>
   </bookViews>
   <sheets>
-    <sheet name="Table1.MLH1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table2.DMC1" sheetId="2" r:id="rId2"/>
+    <sheet name="Table.Strain.Info" sheetId="3" r:id="rId1"/>
+    <sheet name="Table1.MLH1" sheetId="1" r:id="rId2"/>
+    <sheet name="Table2.DMC1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,8 +25,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>April Peterson</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>April Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This table could list the strains with these columns:
+Subspecies/Species 
+Strain
+Geographic Origin
+Source
+First list subspecies of house mice (keeping strains of the same subspecies together), then other murid species. Alphabetical by strain within subspecies.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t>Species</t>
   </si>
@@ -148,13 +189,103 @@
   </si>
   <si>
     <t>Number of Mice</t>
+  </si>
+  <si>
+    <t>subspecies</t>
+  </si>
+  <si>
+    <t>strain</t>
+  </si>
+  <si>
+    <t>geo-origin</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Dom</t>
+  </si>
+  <si>
+    <t>Musc</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>CZECHII</t>
+  </si>
+  <si>
+    <t>central Europe, Czech</t>
+  </si>
+  <si>
+    <t>Kazatstan</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Jackson Lab</t>
+  </si>
+  <si>
+    <t>RIKEN</t>
+  </si>
+  <si>
+    <t>Gough Island</t>
+  </si>
+  <si>
+    <t>Mol</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Spicilegus</t>
+  </si>
+  <si>
+    <t>Caroli</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>CAST</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Thailand?</t>
+  </si>
+  <si>
+    <t>PERC</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>East Coast USA</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>TOM</t>
+  </si>
+  <si>
+    <t>Paysuer Lab</t>
+  </si>
+  <si>
+    <t>Western Europe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +309,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -368,47 +520,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -429,9 +551,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -442,9 +561,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,33 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -517,6 +606,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,6 +949,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J22"/>
   <sheetViews>
@@ -811,586 +1187,586 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="32" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>184</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="12">
         <v>24.701000000000001</v>
       </c>
-      <c r="H3" s="42">
+      <c r="H3" s="21">
         <v>0.26700000000000002</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="22">
         <v>14.638271224837814</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="21">
         <v>13.074</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="56" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="3">
         <v>11</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="3">
         <v>222</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="8">
         <v>23.382999999999999</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="23">
         <v>0.18</v>
       </c>
-      <c r="I4" s="45">
+      <c r="I4" s="24">
         <v>11.479933887268658</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="23">
         <v>7.2060000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="3">
         <v>12</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="3">
         <v>318</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="8">
         <v>28.210999999999999</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="23">
         <v>0.23499999999999999</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="24">
         <v>14.835969061582837</v>
       </c>
-      <c r="J5" s="44">
+      <c r="J5" s="23">
         <v>17.516999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="57" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="3">
         <v>18</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="3">
         <v>355</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="8">
         <v>23.161000000000001</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="23">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="24">
         <v>11.35380583435758</v>
       </c>
-      <c r="J6" s="44">
+      <c r="J6" s="23">
         <v>6.915</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="3">
         <v>9</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="3">
         <v>147</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="8">
         <v>26.585000000000001</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="23">
         <v>0.39800000000000002</v>
       </c>
-      <c r="I7" s="45">
+      <c r="I7" s="24">
         <v>18.16189516714001</v>
       </c>
-      <c r="J7" s="44">
+      <c r="J7" s="23">
         <v>23.312999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="57" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="4">
         <v>10</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="4">
         <v>253</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="16">
         <v>24.161999999999999</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="25">
         <v>0.19500000000000001</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="26">
         <v>12.83701437670674</v>
       </c>
-      <c r="J8" s="46">
+      <c r="J8" s="25">
         <v>9.6199999999999992</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>15</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>222</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="12">
         <v>25.977</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="21">
         <v>0.251</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="22">
         <v>14.41018621027294</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="21">
         <v>14.013</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="56" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="3">
         <v>8</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="3">
         <v>161</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="8">
         <v>28.670999999999999</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="23">
         <v>0.246</v>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="24">
         <v>10.896284161204306</v>
       </c>
-      <c r="J10" s="44">
+      <c r="J10" s="23">
         <v>9.76</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="3">
         <v>32</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="8">
         <v>25.937999999999999</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="23">
         <v>0.55300000000000005</v>
       </c>
-      <c r="I11" s="45">
+      <c r="I11" s="24">
         <v>12.070868672504577</v>
       </c>
-      <c r="J11" s="44">
+      <c r="J11" s="23">
         <v>9.8019999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="57" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="3">
         <v>3</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="3">
         <v>86</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="8">
         <v>26.081</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="23">
         <v>0.29299999999999998</v>
       </c>
-      <c r="I12" s="45">
+      <c r="I12" s="24">
         <v>10.408689886052935</v>
       </c>
-      <c r="J12" s="44">
+      <c r="J12" s="23">
         <v>7.37</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="3">
         <v>9</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="3">
         <v>184</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="8">
         <v>25.625</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="23">
         <v>0.29499999999999998</v>
       </c>
-      <c r="I13" s="45">
+      <c r="I13" s="24">
         <v>15.628736960600049</v>
       </c>
-      <c r="J13" s="44">
+      <c r="J13" s="23">
         <v>16.039000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="57" t="s">
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="4">
         <v>13</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="4">
         <v>264</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="16">
         <v>22.989000000000001</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="25">
         <v>0.186</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="26">
         <v>13.159636243359548</v>
       </c>
-      <c r="J14" s="46">
+      <c r="J14" s="25">
         <v>9.1519999999999992</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>14</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="2">
         <v>300</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="12">
         <v>28.123000000000001</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="21">
         <v>0.254</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="27">
         <v>15.64239374084605</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="21">
         <v>19.353000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="56" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="3">
         <v>7</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="3">
         <v>166</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="8">
         <v>30.367000000000001</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="23">
         <v>0.24199999999999999</v>
       </c>
-      <c r="I16" s="49">
+      <c r="I16" s="28">
         <v>10.262658213499735</v>
       </c>
-      <c r="J16" s="46">
+      <c r="J16" s="25">
         <v>9.7129999999999992</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="3">
         <v>21</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="8">
         <v>27.619</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="23">
         <v>0.92400000000000004</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="23">
         <v>15.338917885642941</v>
       </c>
-      <c r="J17" s="50">
+      <c r="J17" s="29">
         <v>17.948</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="57" t="s">
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="4">
         <v>6</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="4">
         <v>119</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="16">
         <v>23.42</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="25">
         <v>0.23200000000000001</v>
       </c>
-      <c r="I18" s="46">
+      <c r="I18" s="25">
         <v>10.80040516644884</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="30">
         <v>6.3979999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="3">
         <v>2</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="8">
         <v>26</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="23">
         <v>2</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="23">
         <v>10.878565864408424</v>
       </c>
-      <c r="J19" s="50">
+      <c r="J19" s="29">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="56" t="s">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="3">
         <v>5</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="3">
         <v>103</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="8">
         <v>24.427</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="23">
         <v>0.246</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="23">
         <v>10.232121984584271</v>
       </c>
-      <c r="J20" s="50">
+      <c r="J20" s="29">
         <v>6.2469999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="55" t="s">
+      <c r="D21" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>6</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="2">
         <v>97</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="12">
         <v>28.236999999999998</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="21">
         <v>0.44800000000000001</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="21">
         <v>15.628316890383017</v>
       </c>
-      <c r="J21" s="52">
+      <c r="J21" s="31">
         <v>19.474</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="57" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="4">
         <v>4</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="4">
         <v>133</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="16">
         <v>25.774000000000001</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="25">
         <v>0.24099999999999999</v>
       </c>
-      <c r="I22" s="46">
+      <c r="I22" s="25">
         <v>10.781039022222362</v>
       </c>
-      <c r="J22" s="51">
+      <c r="J22" s="30">
         <v>7.7210000000000001</v>
       </c>
     </row>
@@ -1417,11 +1793,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1437,166 +1813,166 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="15" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="7">
         <v>21</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="8">
         <v>177.76190476190476</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="9">
         <v>0.13715946228965248</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="10">
         <v>20</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="8">
         <v>144.25</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="9">
         <v>0.16902410587679217</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="7">
         <v>19</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="8">
         <v>158.15789473684211</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="9">
         <v>0.15299197633573675</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="10">
         <v>9</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="8">
         <v>131.77777777777777</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="9">
         <v>0.18361888701517706</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="53"/>
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="8">
         <v>159</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="9">
         <v>0.15241074020319303</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="10">
         <v>11</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="8">
         <v>167.36363636363637</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="9">
         <v>0.1447943425395897</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="11">
         <v>18</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <v>180.22222222222223</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="13">
         <v>0.16261243834771885</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="14">
         <v>18</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="12">
         <v>140.77777777777777</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="13">
         <v>0.20817472375690607</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="55"/>
+      <c r="B8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="15">
         <v>17</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="16">
         <v>231</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="17">
         <v>0.13518614718614719</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="18">
         <v>17</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="16">
         <v>164.41176470588235</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="17">
         <v>0.1899377459749553</v>
       </c>
     </row>

</xml_diff>